<commit_message>
structure excel file amended
</commit_message>
<xml_diff>
--- a/public/docs/TwoThousands.xlsx
+++ b/public/docs/TwoThousands.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\01_WebDevelop\01_FullStack\04_TeachLearnFront\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858C8FD9-4096-43A0-8233-F8A73C4FFB01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA97924F-B6F1-4AD6-8430-81FF4B95DD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
+    <workbookView xWindow="-28920" yWindow="-8985" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{3025596F-8F86-4685-8931-8FCF7E89A1B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="4" r:id="rId1"/>
     <sheet name="Words" sheetId="3" r:id="rId2"/>
     <sheet name="Sentences" sheetId="6" r:id="rId3"/>
     <sheet name="Grammar" sheetId="8" r:id="rId4"/>
+    <sheet name="Topics" sheetId="9" r:id="rId5"/>
+    <sheet name="LessonStructure" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11354" uniqueCount="4773">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11467" uniqueCount="4833">
   <si>
     <t>з</t>
   </si>
@@ -14358,13 +14360,193 @@
   </si>
   <si>
     <t>"},</t>
+  </si>
+  <si>
+    <t>TOPICS</t>
+  </si>
+  <si>
+    <t>Introductions &amp; Personal Information – Talk about yourself, your background, and your interests.</t>
+  </si>
+  <si>
+    <t>Daily Routines – Describe your typical day from morning to night.</t>
+  </si>
+  <si>
+    <t>Hobbies &amp; Free Time – Discuss your favorite activities, sports, or creative pursuits.</t>
+  </si>
+  <si>
+    <t>Travel &amp; Holidays – Share experiences about past trips or dream destinations.</t>
+  </si>
+  <si>
+    <t>Food &amp; Cooking – Talk about favorite dishes, recipes, and eating habits.</t>
+  </si>
+  <si>
+    <t>Family &amp; Friends – Describe your relationships and social life.</t>
+  </si>
+  <si>
+    <t>School &amp; Education – Discuss school experiences, favorite subjects, and learning methods.</t>
+  </si>
+  <si>
+    <t>Work &amp; Careers – Talk about jobs, career goals, and workplace culture.</t>
+  </si>
+  <si>
+    <t>Shopping &amp; Money – Discuss buying habits, budgeting, and favorite stores.</t>
+  </si>
+  <si>
+    <t>Technology &amp; Social Media – Talk about how you use technology and its effects on daily life.</t>
+  </si>
+  <si>
+    <t>Movies &amp; TV Shows – Share opinions on films, series, and actors.</t>
+  </si>
+  <si>
+    <t>Music &amp; Entertainment – Talk about favorite musicians, concerts, and music genres.</t>
+  </si>
+  <si>
+    <t>Sports &amp; Exercise – Discuss favorite sports, fitness routines, and staying healthy.</t>
+  </si>
+  <si>
+    <t>News &amp; Current Events – Share thoughts on recent world events and local news.</t>
+  </si>
+  <si>
+    <t>Dreams &amp; Future Plans – Talk about life goals, ambitions, and hopes for the future.</t>
+  </si>
+  <si>
+    <t>Cultural Differences – Discuss traditions, customs, and cultural experiences.</t>
+  </si>
+  <si>
+    <t>Weather &amp; Seasons – Talk about favorite seasons and how weather affects daily life.</t>
+  </si>
+  <si>
+    <t>Health &amp; Wellness – Discuss habits for staying healthy and dealing with stress.</t>
+  </si>
+  <si>
+    <t>Personal Experiences &amp; Stories – Share interesting life events or funny stories.</t>
+  </si>
+  <si>
+    <t>If You Could... – Imagine different scenarios like "If you could travel anywhere, where would you go?"</t>
+  </si>
+  <si>
+    <t>VOCABULARY</t>
+  </si>
+  <si>
+    <t>Reading all words</t>
+  </si>
+  <si>
+    <t>Meaning of some words</t>
+  </si>
+  <si>
+    <t>GRAMMAR</t>
+  </si>
+  <si>
+    <t>Topic: tables, images, graphs etc.</t>
+  </si>
+  <si>
+    <t>Exercise type 1 - translate words in bold</t>
+  </si>
+  <si>
+    <t>Exercise type 2 - translation from Ukrainian</t>
+  </si>
+  <si>
+    <t>Exercise type 3 - transformation</t>
+  </si>
+  <si>
+    <t>READING (words &amp; topic)</t>
+  </si>
+  <si>
+    <t>Sentences</t>
+  </si>
+  <si>
+    <t>Little story on the topic</t>
+  </si>
+  <si>
+    <t>Five questions about story</t>
+  </si>
+  <si>
+    <t>LISTENING (words &amp; topic)</t>
+  </si>
+  <si>
+    <t>Three small texts on the topic - audio/video</t>
+  </si>
+  <si>
+    <t>Brief content of the text in Ukrainian</t>
+  </si>
+  <si>
+    <t>SPEAKING (words &amp; topic)</t>
+  </si>
+  <si>
+    <t>Dialogue</t>
+  </si>
+  <si>
+    <t>Small text from Ukrainian to English</t>
+  </si>
+  <si>
+    <t>Vocabulary</t>
+  </si>
+  <si>
+    <t>Grammar rules</t>
+  </si>
+  <si>
+    <t>Grammar replace it</t>
+  </si>
+  <si>
+    <t>Grammar fix it</t>
+  </si>
+  <si>
+    <t>Grammar fill it in</t>
+  </si>
+  <si>
+    <t>Reading text and questions</t>
+  </si>
+  <si>
+    <t>Reading signs</t>
+  </si>
+  <si>
+    <t>Listening text and questions #1</t>
+  </si>
+  <si>
+    <t>Listening text and questions #2</t>
+  </si>
+  <si>
+    <t>Speaking dialog</t>
+  </si>
+  <si>
+    <t>Speaking story</t>
+  </si>
+  <si>
+    <t>from 2 thousands</t>
+  </si>
+  <si>
+    <t>Continuous tense</t>
+  </si>
+  <si>
+    <t>Time and dates</t>
+  </si>
+  <si>
+    <t>There is/there are, Articles</t>
+  </si>
+  <si>
+    <t>Singular and Plural nouns, Comparative and Superlative Adjectives</t>
+  </si>
+  <si>
+    <t>Modal verbs, Would and Used to</t>
+  </si>
+  <si>
+    <t>Pronouns, To be</t>
+  </si>
+  <si>
+    <t>Reading rules</t>
+  </si>
+  <si>
+    <t>GRAMMAR TOPICS</t>
+  </si>
+  <si>
+    <t>from Grammar Topics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -14392,6 +14574,12 @@
       <sz val="8"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -14459,7 +14647,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -24111,7 +24299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA00D292-BF8B-4F4B-B7D2-0977FA8E2544}">
   <dimension ref="A1:F2192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1983" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A1983" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G1988" sqref="G1988"/>
     </sheetView>
   </sheetViews>
@@ -71106,24 +71294,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2065B795-6495-421C-8C31-54BC300F0CEC}">
-  <dimension ref="A2:D42"/>
+  <dimension ref="A2:J42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="I2" sqref="I2:J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="49.6640625" customWidth="1"/>
     <col min="3" max="3" width="46.77734375" customWidth="1"/>
+    <col min="10" max="10" width="62.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>4769</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>4829</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -71134,8 +71329,14 @@
         <f>"    - "&amp;B3</f>
         <v xml:space="preserve">    - Pronouns</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>4830</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -71146,8 +71347,14 @@
         <f t="shared" ref="C4:C42" si="0">"    - "&amp;B4</f>
         <v xml:space="preserve">    - To be</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>4729</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -71158,8 +71365,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Present simple</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>4758</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -71170,8 +71383,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Future simple</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4759</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -71182,8 +71401,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Past simple</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>4731</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -71194,8 +71419,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Irregular verbs</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>4761</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -71206,8 +71437,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Simple Tense</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>4824</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -71218,8 +71455,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Negative and interrogative sentences - Simple</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>4762</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -71230,8 +71473,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Present Continuous</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>4730</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -71242,8 +71491,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Future Continuous</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>11</v>
+      </c>
+      <c r="J12" t="s">
+        <v>4738</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -71254,8 +71509,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Past Continuous</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>12</v>
+      </c>
+      <c r="J13" t="s">
+        <v>4732</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -71266,8 +71527,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Continuous Tense</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="J14" t="s">
+        <v>4825</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -71278,8 +71545,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Negative and interrogative sentences - Continuous</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>4826</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -71290,8 +71563,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Present Perfect</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>15</v>
+      </c>
+      <c r="J16" t="s">
+        <v>4827</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -71302,8 +71581,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - All Tenses</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>16</v>
+      </c>
+      <c r="J17" t="s">
+        <v>4740</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -71314,8 +71599,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Negative and interrogative sentences - All Tenses</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>17</v>
+      </c>
+      <c r="J18" t="s">
+        <v>4828</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -71326,8 +71617,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Prepositions of place</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <v>18</v>
+      </c>
+      <c r="J19" t="s">
+        <v>4743</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -71338,8 +71635,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - What is the time</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <v>19</v>
+      </c>
+      <c r="J20" t="s">
+        <v>4754</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -71350,8 +71653,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Dates in English</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I21">
+        <v>20</v>
+      </c>
+      <c r="J21" t="s">
+        <v>4755</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -71362,8 +71671,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - There is/there are</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <v>21</v>
+      </c>
+      <c r="J22" t="s">
+        <v>4746</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -71374,8 +71689,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Articles</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I23">
+        <v>22</v>
+      </c>
+      <c r="J23" t="s">
+        <v>4745</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -71386,8 +71707,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Singular and Plural nouns</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I24">
+        <v>23</v>
+      </c>
+      <c r="J24" t="s">
+        <v>4753</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -71398,8 +71725,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Comparative and Superlative Adjectives</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I25">
+        <v>24</v>
+      </c>
+      <c r="J25" t="s">
+        <v>4768</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -71410,8 +71743,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Active Voice and Passive Voice</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I26">
+        <v>25</v>
+      </c>
+      <c r="J26" t="s">
+        <v>4747</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -71422,8 +71761,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Modal verbs</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I27">
+        <v>26</v>
+      </c>
+      <c r="J27" t="s">
+        <v>4748</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -71434,8 +71779,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Would and Used to</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I28">
+        <v>27</v>
+      </c>
+      <c r="J28" t="s">
+        <v>4751</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -71446,8 +71797,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - Imperative sentences</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I29">
+        <v>28</v>
+      </c>
+      <c r="J29" t="s">
+        <v>4750</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -71461,8 +71818,14 @@
       <c r="D30" t="s">
         <v>4744</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I30">
+        <v>29</v>
+      </c>
+      <c r="J30" t="s">
+        <v>4752</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -71473,8 +71836,14 @@
         <f t="shared" si="0"/>
         <v xml:space="preserve">    - 8 basic rules of Grammar (part 2)</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="I31">
+        <v>30</v>
+      </c>
+      <c r="J31" t="s">
+        <v>4757</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -71610,4 +71979,548 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95E59B5-B434-461C-8003-542FC86AE77F}">
+  <dimension ref="B2:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="98.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>4773</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4774</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4775</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4776</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4777</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4778</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4779</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4780</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4781</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4782</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4783</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4784</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4785</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4786</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4787</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4788</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4789</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4790</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4791</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4792</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4793</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3283C63A-6C75-489B-8AE0-6D8190C9BE6E}">
+  <dimension ref="C1:O31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="36.77734375" customWidth="1"/>
+    <col min="8" max="8" width="28.6640625" customWidth="1"/>
+    <col min="9" max="9" width="37.6640625" customWidth="1"/>
+    <col min="14" max="14" width="8.77734375" customWidth="1"/>
+    <col min="15" max="15" width="57.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="O1" s="6" t="s">
+        <v>4831</v>
+      </c>
+    </row>
+    <row r="2" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C2" s="6" t="s">
+        <v>4794</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>4829</v>
+      </c>
+    </row>
+    <row r="3" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>4795</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4812</v>
+      </c>
+      <c r="I3" t="s">
+        <v>4823</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3" t="s">
+        <v>4830</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>4796</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4813</v>
+      </c>
+      <c r="I4" t="s">
+        <v>4832</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4" t="s">
+        <v>4729</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>4814</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5" t="s">
+        <v>4758</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C6" s="6" t="s">
+        <v>4797</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4815</v>
+      </c>
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="O6" t="s">
+        <v>4759</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>4798</v>
+      </c>
+      <c r="H7" t="s">
+        <v>4816</v>
+      </c>
+      <c r="N7">
+        <v>6</v>
+      </c>
+      <c r="O7" t="s">
+        <v>4731</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>4799</v>
+      </c>
+      <c r="H8" t="s">
+        <v>4817</v>
+      </c>
+      <c r="N8">
+        <v>7</v>
+      </c>
+      <c r="O8" t="s">
+        <v>4761</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>4800</v>
+      </c>
+      <c r="H9" t="s">
+        <v>4818</v>
+      </c>
+      <c r="N9">
+        <v>8</v>
+      </c>
+      <c r="O9" t="s">
+        <v>4824</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>4801</v>
+      </c>
+      <c r="H10" t="s">
+        <v>4819</v>
+      </c>
+      <c r="N10">
+        <v>9</v>
+      </c>
+      <c r="O10" t="s">
+        <v>4762</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>4820</v>
+      </c>
+      <c r="N11">
+        <v>10</v>
+      </c>
+      <c r="O11" t="s">
+        <v>4730</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C12" s="6" t="s">
+        <v>4802</v>
+      </c>
+      <c r="H12" t="s">
+        <v>4821</v>
+      </c>
+      <c r="N12">
+        <v>11</v>
+      </c>
+      <c r="O12" t="s">
+        <v>4738</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>4803</v>
+      </c>
+      <c r="H13" t="s">
+        <v>4822</v>
+      </c>
+      <c r="N13">
+        <v>12</v>
+      </c>
+      <c r="O13" t="s">
+        <v>4732</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>4804</v>
+      </c>
+      <c r="N14">
+        <v>13</v>
+      </c>
+      <c r="O14" t="s">
+        <v>4825</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>4805</v>
+      </c>
+      <c r="N15">
+        <v>14</v>
+      </c>
+      <c r="O15" t="s">
+        <v>4826</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="N16">
+        <v>15</v>
+      </c>
+      <c r="O16" t="s">
+        <v>4827</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C17" s="6" t="s">
+        <v>4806</v>
+      </c>
+      <c r="N17">
+        <v>16</v>
+      </c>
+      <c r="O17" t="s">
+        <v>4740</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>4807</v>
+      </c>
+      <c r="N18">
+        <v>17</v>
+      </c>
+      <c r="O18" t="s">
+        <v>4828</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>4808</v>
+      </c>
+      <c r="N19">
+        <v>18</v>
+      </c>
+      <c r="O19" t="s">
+        <v>4743</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="N20">
+        <v>19</v>
+      </c>
+      <c r="O20" t="s">
+        <v>4754</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C21" s="6" t="s">
+        <v>4809</v>
+      </c>
+      <c r="N21">
+        <v>20</v>
+      </c>
+      <c r="O21" t="s">
+        <v>4755</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>4810</v>
+      </c>
+      <c r="N22">
+        <v>21</v>
+      </c>
+      <c r="O22" t="s">
+        <v>4746</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>4811</v>
+      </c>
+      <c r="N23">
+        <v>22</v>
+      </c>
+      <c r="O23" t="s">
+        <v>4745</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="N24">
+        <v>23</v>
+      </c>
+      <c r="O24" t="s">
+        <v>4753</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="N25">
+        <v>24</v>
+      </c>
+      <c r="O25" t="s">
+        <v>4768</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="N26">
+        <v>25</v>
+      </c>
+      <c r="O26" t="s">
+        <v>4747</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="N27">
+        <v>26</v>
+      </c>
+      <c r="O27" t="s">
+        <v>4748</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="N28">
+        <v>27</v>
+      </c>
+      <c r="O28" t="s">
+        <v>4751</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="N29">
+        <v>28</v>
+      </c>
+      <c r="O29" t="s">
+        <v>4750</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="N30">
+        <v>29</v>
+      </c>
+      <c r="O30" t="s">
+        <v>4752</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.3">
+      <c r="N31">
+        <v>30</v>
+      </c>
+      <c r="O31" t="s">
+        <v>4757</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>